<commit_message>
Update council vaccinations data
</commit_message>
<xml_diff>
--- a/src/data/lga-vaccinations/source.xlsx
+++ b/src/data/lga-vaccinations/source.xlsx
@@ -5,20 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\central.health\dfsuserenv\Users\User_24\JACREU\Documents\In progress\Afternoon\13.12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\central.health\dfsuserenv\Users\User_24\JACREU\Documents\In progress\Afternoon\20.12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD933FA4-468F-49F5-A948-A8D8297D4405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50512A2B-4958-4666-9423-ADBCD44F7A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="2145" windowWidth="20850" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LGA vaccine data 13 Dec 2021" sheetId="1" r:id="rId1"/>
+    <sheet name="LGA Vaccine data 20 Dec 21" sheetId="1" r:id="rId1"/>
     <sheet name="Remoteness" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'LGA vaccine data 13 Dec 2021'!$A$1:$F$552</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">RemotenessTable[#All]</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'LGA Vaccine data 20 Dec 21'!$A$1:$F$552</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3272" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3272" uniqueCount="769">
   <si>
     <t>LGA 2019 Name of Residence</t>
   </si>
@@ -1702,7 +1701,7 @@
     <t>LGA Name</t>
   </si>
   <si>
-    <t>Data extracted from AIR - as at 2359hrs on 12 December 2021</t>
+    <t>Data extracted from AIR - as at 2359hrs on 19 December 2021</t>
   </si>
   <si>
     <t>Cherbourg (S)*</t>
@@ -1851,613 +1850,571 @@
     <t>&gt;95%</t>
   </si>
   <si>
+    <t>91.8%</t>
+  </si>
+  <si>
+    <t>94.2%</t>
+  </si>
+  <si>
+    <t>91.0%</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>91.1%</t>
+  </si>
+  <si>
+    <t>93.9%</t>
+  </si>
+  <si>
+    <t>88.0%</t>
+  </si>
+  <si>
+    <t>86.9%</t>
+  </si>
+  <si>
+    <t>93.6%</t>
+  </si>
+  <si>
+    <t>69.8%</t>
+  </si>
+  <si>
+    <t>90.9%</t>
+  </si>
+  <si>
+    <t>92.5%</t>
+  </si>
+  <si>
+    <t>89.7%</t>
+  </si>
+  <si>
+    <t>83.4%</t>
+  </si>
+  <si>
+    <t>85.3%</t>
+  </si>
+  <si>
+    <t>92.7%</t>
+  </si>
+  <si>
+    <t>91.4%</t>
+  </si>
+  <si>
+    <t>94.5%</t>
+  </si>
+  <si>
+    <t>94.6%</t>
+  </si>
+  <si>
+    <t>85.7%</t>
+  </si>
+  <si>
+    <t>82.1%</t>
+  </si>
+  <si>
+    <t>92.6%</t>
+  </si>
+  <si>
+    <t>93.0%</t>
+  </si>
+  <si>
+    <t>75.8%</t>
+  </si>
+  <si>
+    <t>92.1%</t>
+  </si>
+  <si>
+    <t>86.7%</t>
+  </si>
+  <si>
+    <t>92.8%</t>
+  </si>
+  <si>
+    <t>90.7%</t>
+  </si>
+  <si>
+    <t>94.4%</t>
+  </si>
+  <si>
+    <t>82.9%</t>
+  </si>
+  <si>
+    <t>93.8%</t>
+  </si>
+  <si>
+    <t>93.1%</t>
+  </si>
+  <si>
+    <t>84.9%</t>
+  </si>
+  <si>
+    <t>76.6%</t>
+  </si>
+  <si>
+    <t>90.3%</t>
+  </si>
+  <si>
+    <t>84.2%</t>
+  </si>
+  <si>
+    <t>80.8%</t>
+  </si>
+  <si>
+    <t>82.6%</t>
+  </si>
+  <si>
+    <t>94.1%</t>
+  </si>
+  <si>
+    <t>77.7%</t>
+  </si>
+  <si>
+    <t>47.1%</t>
+  </si>
+  <si>
+    <t>83.7%</t>
+  </si>
+  <si>
+    <t>90.5%</t>
+  </si>
+  <si>
+    <t>94.8%</t>
+  </si>
+  <si>
+    <t>92.4%</t>
+  </si>
+  <si>
+    <t>90.1%</t>
+  </si>
+  <si>
+    <t>82.5%</t>
+  </si>
+  <si>
+    <t>63.5%</t>
+  </si>
+  <si>
+    <t>89.3%</t>
+  </si>
+  <si>
+    <t>89.8%</t>
+  </si>
+  <si>
+    <t>88.9%</t>
+  </si>
+  <si>
+    <t>87.0%</t>
+  </si>
+  <si>
+    <t>71.8%</t>
+  </si>
+  <si>
+    <t>87.5%</t>
+  </si>
+  <si>
+    <t>85.9%</t>
+  </si>
+  <si>
+    <t>90.4%</t>
+  </si>
+  <si>
+    <t>81.3%</t>
+  </si>
+  <si>
+    <t>87.7%</t>
+  </si>
+  <si>
+    <t>93.5%</t>
+  </si>
+  <si>
+    <t>89.0%</t>
+  </si>
+  <si>
+    <t>89.5%</t>
+  </si>
+  <si>
+    <t>89.4%</t>
+  </si>
+  <si>
+    <t>88.7%</t>
+  </si>
+  <si>
+    <t>71.6%</t>
+  </si>
+  <si>
+    <t>85.4%</t>
+  </si>
+  <si>
+    <t>88.2%</t>
+  </si>
+  <si>
+    <t>83.1%</t>
+  </si>
+  <si>
+    <t>80.2%</t>
+  </si>
+  <si>
+    <t>78.9%</t>
+  </si>
+  <si>
+    <t>79.4%</t>
+  </si>
+  <si>
+    <t>80.4%</t>
+  </si>
+  <si>
+    <t>93.4%</t>
+  </si>
+  <si>
+    <t>92.0%</t>
+  </si>
+  <si>
+    <t>85.0%</t>
+  </si>
+  <si>
+    <t>90.8%</t>
+  </si>
+  <si>
+    <t>91.6%</t>
+  </si>
+  <si>
+    <t>94.3%</t>
+  </si>
+  <si>
+    <t>88.3%</t>
+  </si>
+  <si>
+    <t>93.3%</t>
+  </si>
+  <si>
+    <t>87.8%</t>
+  </si>
+  <si>
+    <t>94.9%</t>
+  </si>
+  <si>
+    <t>91.2%</t>
+  </si>
+  <si>
+    <t>87.6%</t>
+  </si>
+  <si>
+    <t>92.9%</t>
+  </si>
+  <si>
     <t>91.7%</t>
   </si>
   <si>
-    <t>94.1%</t>
-  </si>
-  <si>
-    <t>90.8%</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>90.9%</t>
+    <t>87.4%</t>
+  </si>
+  <si>
+    <t>86.2%</t>
+  </si>
+  <si>
+    <t>80.7%</t>
+  </si>
+  <si>
+    <t>85.2%</t>
+  </si>
+  <si>
+    <t>77.9%</t>
+  </si>
+  <si>
+    <t>62.4%</t>
+  </si>
+  <si>
+    <t>77.6%</t>
+  </si>
+  <si>
+    <t>85.6%</t>
+  </si>
+  <si>
+    <t>88.8%</t>
+  </si>
+  <si>
+    <t>80.1%</t>
+  </si>
+  <si>
+    <t>79.2%</t>
+  </si>
+  <si>
+    <t>92.3%</t>
+  </si>
+  <si>
+    <t>94.0%</t>
+  </si>
+  <si>
+    <t>86.1%</t>
+  </si>
+  <si>
+    <t>83.0%</t>
+  </si>
+  <si>
+    <t>93.2%</t>
+  </si>
+  <si>
+    <t>91.3%</t>
+  </si>
+  <si>
+    <t>89.6%</t>
+  </si>
+  <si>
+    <t>89.2%</t>
+  </si>
+  <si>
+    <t>85.8%</t>
+  </si>
+  <si>
+    <t>79.8%</t>
+  </si>
+  <si>
+    <t>92.2%</t>
+  </si>
+  <si>
+    <t>86.8%</t>
+  </si>
+  <si>
+    <t>87.1%</t>
+  </si>
+  <si>
+    <t>84.3%</t>
+  </si>
+  <si>
+    <t>84.4%</t>
+  </si>
+  <si>
+    <t>90.2%</t>
+  </si>
+  <si>
+    <t>89.9%</t>
+  </si>
+  <si>
+    <t>87.3%</t>
+  </si>
+  <si>
+    <t>72.8%</t>
+  </si>
+  <si>
+    <t>90.0%</t>
   </si>
   <si>
     <t>93.7%</t>
   </si>
   <si>
-    <t>87.7%</t>
-  </si>
-  <si>
-    <t>86.8%</t>
-  </si>
-  <si>
-    <t>93.5%</t>
-  </si>
-  <si>
-    <t>69.6%</t>
-  </si>
-  <si>
-    <t>92.4%</t>
-  </si>
-  <si>
-    <t>89.6%</t>
-  </si>
-  <si>
-    <t>83.4%</t>
-  </si>
-  <si>
-    <t>85.3%</t>
-  </si>
-  <si>
-    <t>93.4%</t>
-  </si>
-  <si>
-    <t>92.6%</t>
-  </si>
-  <si>
-    <t>91.2%</t>
-  </si>
-  <si>
-    <t>94.2%</t>
-  </si>
-  <si>
-    <t>94.5%</t>
-  </si>
-  <si>
-    <t>85.6%</t>
+    <t>91.5%</t>
+  </si>
+  <si>
+    <t>66.5%</t>
+  </si>
+  <si>
+    <t>94.7%</t>
+  </si>
+  <si>
+    <t>68.4%</t>
+  </si>
+  <si>
+    <t>82.4%</t>
+  </si>
+  <si>
+    <t>84.0%</t>
+  </si>
+  <si>
+    <t>88.4%</t>
+  </si>
+  <si>
+    <t>84.8%</t>
+  </si>
+  <si>
+    <t>74.4%</t>
+  </si>
+  <si>
+    <t>95.0%</t>
+  </si>
+  <si>
+    <t>81.4%</t>
+  </si>
+  <si>
+    <t>91.9%</t>
+  </si>
+  <si>
+    <t>74.8%</t>
+  </si>
+  <si>
+    <t>88.5%</t>
+  </si>
+  <si>
+    <t>79.5%</t>
+  </si>
+  <si>
+    <t>81.6%</t>
+  </si>
+  <si>
+    <t>46.2%</t>
+  </si>
+  <si>
+    <t>74.1%</t>
+  </si>
+  <si>
+    <t>73.9%</t>
+  </si>
+  <si>
+    <t>52.8%</t>
+  </si>
+  <si>
+    <t>84.7%</t>
+  </si>
+  <si>
+    <t>84.1%</t>
+  </si>
+  <si>
+    <t>81.0%</t>
+  </si>
+  <si>
+    <t>79.7%</t>
+  </si>
+  <si>
+    <t>83.3%</t>
+  </si>
+  <si>
+    <t>73.5%</t>
+  </si>
+  <si>
+    <t>78.7%</t>
+  </si>
+  <si>
+    <t>82.3%</t>
+  </si>
+  <si>
+    <t>83.2%</t>
+  </si>
+  <si>
+    <t>83.9%</t>
+  </si>
+  <si>
+    <t>81.8%</t>
+  </si>
+  <si>
+    <t>56.9%</t>
+  </si>
+  <si>
+    <t>78.6%</t>
+  </si>
+  <si>
+    <t>88.6%</t>
+  </si>
+  <si>
+    <t>77.2%</t>
+  </si>
+  <si>
+    <t>76.3%</t>
+  </si>
+  <si>
+    <t>74.0%</t>
+  </si>
+  <si>
+    <t>77.3%</t>
+  </si>
+  <si>
+    <t>90.6%</t>
+  </si>
+  <si>
+    <t>78.8%</t>
+  </si>
+  <si>
+    <t>89.1%</t>
   </si>
   <si>
     <t>82.0%</t>
   </si>
   <si>
-    <t>92.5%</t>
-  </si>
-  <si>
-    <t>93.0%</t>
-  </si>
-  <si>
-    <t>75.7%</t>
-  </si>
-  <si>
-    <t>92.0%</t>
-  </si>
-  <si>
-    <t>86.6%</t>
-  </si>
-  <si>
-    <t>92.7%</t>
-  </si>
-  <si>
-    <t>90.5%</t>
-  </si>
-  <si>
-    <t>94.3%</t>
-  </si>
-  <si>
-    <t>90.7%</t>
-  </si>
-  <si>
-    <t>82.8%</t>
-  </si>
-  <si>
-    <t>91.0%</t>
-  </si>
-  <si>
-    <t>93.8%</t>
-  </si>
-  <si>
-    <t>93.1%</t>
-  </si>
-  <si>
-    <t>84.8%</t>
-  </si>
-  <si>
-    <t>94.4%</t>
+    <t>84.5%</t>
+  </si>
+  <si>
+    <t>83.5%</t>
+  </si>
+  <si>
+    <t>71.9%</t>
   </si>
   <si>
     <t>76.5%</t>
   </si>
   <si>
-    <t>90.1%</t>
-  </si>
-  <si>
-    <t>84.1%</t>
-  </si>
-  <si>
-    <t>80.7%</t>
-  </si>
-  <si>
-    <t>82.5%</t>
-  </si>
-  <si>
-    <t>93.9%</t>
-  </si>
-  <si>
-    <t>77.6%</t>
-  </si>
-  <si>
-    <t>46.9%</t>
+    <t>68.2%</t>
+  </si>
+  <si>
+    <t>88.1%</t>
+  </si>
+  <si>
+    <t>83.6%</t>
+  </si>
+  <si>
+    <t>55.3%</t>
+  </si>
+  <si>
+    <t>75.2%</t>
+  </si>
+  <si>
+    <t>65.9%</t>
+  </si>
+  <si>
+    <t>79.0%</t>
+  </si>
+  <si>
+    <t>72.3%</t>
+  </si>
+  <si>
+    <t>87.9%</t>
+  </si>
+  <si>
+    <t>70.9%</t>
+  </si>
+  <si>
+    <t>78.2%</t>
+  </si>
+  <si>
+    <t>77.5%</t>
+  </si>
+  <si>
+    <t>72.7%</t>
+  </si>
+  <si>
+    <t>82.7%</t>
+  </si>
+  <si>
+    <t>80.0%</t>
+  </si>
+  <si>
+    <t>77.0%</t>
+  </si>
+  <si>
+    <t>76.7%</t>
   </si>
   <si>
     <t>81.9%</t>
   </si>
   <si>
-    <t>92.2%</t>
-  </si>
-  <si>
-    <t>90.4%</t>
-  </si>
-  <si>
-    <t>88.3%</t>
-  </si>
-  <si>
-    <t>80.6%</t>
-  </si>
-  <si>
-    <t>80.1%</t>
-  </si>
-  <si>
-    <t>62.0%</t>
-  </si>
-  <si>
-    <t>87.9%</t>
-  </si>
-  <si>
-    <t>87.8%</t>
-  </si>
-  <si>
-    <t>87.5%</t>
-  </si>
-  <si>
-    <t>85.5%</t>
-  </si>
-  <si>
-    <t>94.8%</t>
-  </si>
-  <si>
-    <t>69.4%</t>
-  </si>
-  <si>
-    <t>85.8%</t>
-  </si>
-  <si>
-    <t>84.3%</t>
-  </si>
-  <si>
-    <t>88.4%</t>
-  </si>
-  <si>
-    <t>92.1%</t>
-  </si>
-  <si>
-    <t>90.2%</t>
+    <t>80.5%</t>
+  </si>
+  <si>
+    <t>76.2%</t>
+  </si>
+  <si>
+    <t>81.5%</t>
   </si>
   <si>
     <t>79.1%</t>
   </si>
   <si>
-    <t>92.9%</t>
-  </si>
-  <si>
-    <t>93.3%</t>
-  </si>
-  <si>
-    <t>82.4%</t>
-  </si>
-  <si>
-    <t>95.0%</t>
-  </si>
-  <si>
-    <t>88.2%</t>
-  </si>
-  <si>
-    <t>86.0%</t>
-  </si>
-  <si>
-    <t>87.4%</t>
-  </si>
-  <si>
-    <t>88.7%</t>
-  </si>
-  <si>
-    <t>92.3%</t>
-  </si>
-  <si>
-    <t>87.0%</t>
-  </si>
-  <si>
-    <t>68.2%</t>
-  </si>
-  <si>
-    <t>93.2%</t>
-  </si>
-  <si>
-    <t>84.4%</t>
-  </si>
-  <si>
-    <t>90.6%</t>
-  </si>
-  <si>
-    <t>79.8%</t>
-  </si>
-  <si>
-    <t>78.4%</t>
-  </si>
-  <si>
-    <t>91.9%</t>
-  </si>
-  <si>
-    <t>78.7%</t>
-  </si>
-  <si>
-    <t>82.3%</t>
-  </si>
-  <si>
-    <t>91.4%</t>
-  </si>
-  <si>
-    <t>84.6%</t>
-  </si>
-  <si>
-    <t>88.1%</t>
-  </si>
-  <si>
-    <t>90.0%</t>
-  </si>
-  <si>
-    <t>94.7%</t>
-  </si>
-  <si>
-    <t>86.2%</t>
-  </si>
-  <si>
-    <t>80.0%</t>
-  </si>
-  <si>
-    <t>83.5%</t>
-  </si>
-  <si>
-    <t>76.1%</t>
-  </si>
-  <si>
-    <t>91.3%</t>
-  </si>
-  <si>
-    <t>61.6%</t>
-  </si>
-  <si>
-    <t>83.0%</t>
-  </si>
-  <si>
-    <t>89.5%</t>
-  </si>
-  <si>
-    <t>76.8%</t>
-  </si>
-  <si>
-    <t>84.7%</t>
-  </si>
-  <si>
-    <t>87.6%</t>
-  </si>
-  <si>
-    <t>79.2%</t>
-  </si>
-  <si>
-    <t>78.6%</t>
-  </si>
-  <si>
-    <t>91.1%</t>
-  </si>
-  <si>
-    <t>91.5%</t>
-  </si>
-  <si>
-    <t>92.8%</t>
-  </si>
-  <si>
-    <t>74.7%</t>
-  </si>
-  <si>
-    <t>89.7%</t>
-  </si>
-  <si>
-    <t>93.6%</t>
-  </si>
-  <si>
-    <t>89.2%</t>
-  </si>
-  <si>
-    <t>81.3%</t>
-  </si>
-  <si>
-    <t>94.0%</t>
-  </si>
-  <si>
-    <t>83.8%</t>
-  </si>
-  <si>
-    <t>86.1%</t>
-  </si>
-  <si>
-    <t>85.7%</t>
-  </si>
-  <si>
-    <t>86.9%</t>
-  </si>
-  <si>
-    <t>83.6%</t>
-  </si>
-  <si>
-    <t>88.5%</t>
-  </si>
-  <si>
     <t>87.2%</t>
   </si>
   <si>
-    <t>86.5%</t>
-  </si>
-  <si>
-    <t>72.2%</t>
-  </si>
-  <si>
-    <t>88.6%</t>
-  </si>
-  <si>
-    <t>86.7%</t>
-  </si>
-  <si>
-    <t>94.6%</t>
-  </si>
-  <si>
-    <t>66.2%</t>
-  </si>
-  <si>
-    <t>89.4%</t>
-  </si>
-  <si>
-    <t>89.1%</t>
-  </si>
-  <si>
-    <t>68.0%</t>
-  </si>
-  <si>
-    <t>90.3%</t>
-  </si>
-  <si>
-    <t>80.2%</t>
-  </si>
-  <si>
-    <t>74.3%</t>
-  </si>
-  <si>
-    <t>89.9%</t>
-  </si>
-  <si>
-    <t>85.2%</t>
-  </si>
-  <si>
-    <t>91.8%</t>
-  </si>
-  <si>
-    <t>81.0%</t>
-  </si>
-  <si>
-    <t>89.0%</t>
-  </si>
-  <si>
-    <t>91.6%</t>
-  </si>
-  <si>
-    <t>83.1%</t>
-  </si>
-  <si>
-    <t>74.5%</t>
-  </si>
-  <si>
-    <t>81.4%</t>
-  </si>
-  <si>
-    <t>76.4%</t>
-  </si>
-  <si>
-    <t>45.6%</t>
-  </si>
-  <si>
-    <t>81.8%</t>
-  </si>
-  <si>
-    <t>78.2%</t>
-  </si>
-  <si>
-    <t>69.0%</t>
-  </si>
-  <si>
-    <t>68.7%</t>
-  </si>
-  <si>
-    <t>49.8%</t>
-  </si>
-  <si>
-    <t>77.2%</t>
-  </si>
-  <si>
-    <t>80.8%</t>
-  </si>
-  <si>
-    <t>76.0%</t>
-  </si>
-  <si>
-    <t>81.7%</t>
-  </si>
-  <si>
-    <t>57.4%</t>
-  </si>
-  <si>
-    <t>76.6%</t>
-  </si>
-  <si>
-    <t>75.9%</t>
-  </si>
-  <si>
-    <t>69.1%</t>
-  </si>
-  <si>
-    <t>85.9%</t>
-  </si>
-  <si>
-    <t>74.2%</t>
-  </si>
-  <si>
-    <t>77.1%</t>
-  </si>
-  <si>
-    <t>78.5%</t>
-  </si>
-  <si>
-    <t>78.8%</t>
-  </si>
-  <si>
-    <t>77.9%</t>
-  </si>
-  <si>
-    <t>76.3%</t>
-  </si>
-  <si>
-    <t>52.6%</t>
-  </si>
-  <si>
-    <t>74.9%</t>
-  </si>
-  <si>
-    <t>88.8%</t>
-  </si>
-  <si>
-    <t>82.6%</t>
-  </si>
-  <si>
-    <t>87.1%</t>
-  </si>
-  <si>
-    <t>86.4%</t>
-  </si>
-  <si>
-    <t>75.2%</t>
-  </si>
-  <si>
-    <t>72.1%</t>
-  </si>
-  <si>
-    <t>71.9%</t>
-  </si>
-  <si>
-    <t>74.6%</t>
-  </si>
-  <si>
-    <t>75.1%</t>
-  </si>
-  <si>
-    <t>77.0%</t>
-  </si>
-  <si>
-    <t>81.2%</t>
-  </si>
-  <si>
-    <t>77.7%</t>
-  </si>
-  <si>
-    <t>80.5%</t>
-  </si>
-  <si>
-    <t>76.9%</t>
-  </si>
-  <si>
-    <t>79.4%</t>
-  </si>
-  <si>
-    <t>69.3%</t>
-  </si>
-  <si>
-    <t>73.7%</t>
-  </si>
-  <si>
-    <t>65.9%</t>
-  </si>
-  <si>
-    <t>85.1%</t>
-  </si>
-  <si>
-    <t>53.8%</t>
-  </si>
-  <si>
-    <t>72.5%</t>
-  </si>
-  <si>
-    <t>62.2%</t>
-  </si>
-  <si>
-    <t>73.1%</t>
-  </si>
-  <si>
-    <t>71.4%</t>
-  </si>
-  <si>
-    <t>81.5%</t>
-  </si>
-  <si>
-    <t>89.8%</t>
-  </si>
-  <si>
-    <t>69.8%</t>
-  </si>
-  <si>
-    <t>83.3%</t>
-  </si>
-  <si>
-    <t>75.0%</t>
-  </si>
-  <si>
-    <t>78.1%</t>
-  </si>
-  <si>
-    <t>84.0%</t>
-  </si>
-  <si>
-    <t>70.1%</t>
-  </si>
-  <si>
-    <t>79.7%</t>
-  </si>
-  <si>
-    <t>83.9%</t>
-  </si>
-  <si>
-    <t>73.4%</t>
+    <t>63.6%</t>
   </si>
   <si>
     <t>82.2%</t>
   </si>
   <si>
-    <t>89.3%</t>
-  </si>
-  <si>
-    <t>62.4%</t>
-  </si>
-  <si>
-    <t>79.6%</t>
-  </si>
-  <si>
-    <t>85.4%</t>
-  </si>
-  <si>
-    <t>79.9%</t>
-  </si>
-  <si>
-    <t>60.7%</t>
+    <t>62.1%</t>
   </si>
 </sst>
 </file>
@@ -3030,8 +2987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1095"/>
   <sheetViews>
-    <sheetView topLeftCell="A540" workbookViewId="0">
-      <selection activeCell="A552" sqref="A1:F552"/>
+    <sheetView tabSelected="1" topLeftCell="A533" workbookViewId="0">
+      <selection activeCell="F552" sqref="A1:F552"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3167,7 +3124,7 @@
         <v>580</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>702</v>
+        <v>629</v>
       </c>
       <c r="F11" s="11">
         <v>25368</v>
@@ -3209,7 +3166,7 @@
         <v>581</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>674</v>
+        <v>625</v>
       </c>
       <c r="F13" s="11">
         <v>1859</v>
@@ -3230,7 +3187,7 @@
         <v>579</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>608</v>
+        <v>597</v>
       </c>
       <c r="F14" s="11">
         <v>35111</v>
@@ -3251,7 +3208,7 @@
         <v>582</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F15" s="11">
         <v>150746</v>
@@ -3356,7 +3313,7 @@
         <v>579</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>685</v>
+        <v>696</v>
       </c>
       <c r="F20" s="11">
         <v>4773</v>
@@ -3482,7 +3439,7 @@
         <v>584</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>703</v>
+        <v>640</v>
       </c>
       <c r="F26" s="11">
         <v>14532</v>
@@ -3503,7 +3460,7 @@
         <v>585</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>659</v>
+        <v>686</v>
       </c>
       <c r="F27" s="11">
         <v>35639</v>
@@ -3524,7 +3481,7 @@
         <v>586</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>655</v>
+        <v>594</v>
       </c>
       <c r="F28" s="11">
         <v>29052</v>
@@ -3545,7 +3502,7 @@
         <v>579</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>615</v>
+        <v>699</v>
       </c>
       <c r="F29" s="11">
         <v>10765</v>
@@ -3608,7 +3565,7 @@
         <v>587</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>691</v>
+        <v>634</v>
       </c>
       <c r="F32" s="11">
         <v>80727</v>
@@ -3629,7 +3586,7 @@
         <v>588</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>584</v>
+        <v>661</v>
       </c>
       <c r="F33" s="11">
         <v>301492</v>
@@ -3881,7 +3838,7 @@
         <v>579</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>643</v>
+        <v>680</v>
       </c>
       <c r="F45" s="11">
         <v>192534</v>
@@ -3944,7 +3901,7 @@
         <v>589</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="F48" s="11">
         <v>7426</v>
@@ -3986,7 +3943,7 @@
         <v>579</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>613</v>
+        <v>658</v>
       </c>
       <c r="F50" s="11">
         <v>172126</v>
@@ -4028,7 +3985,7 @@
         <v>579</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>700</v>
+        <v>623</v>
       </c>
       <c r="F52" s="11">
         <v>7865</v>
@@ -4046,10 +4003,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>686</v>
+        <v>641</v>
       </c>
       <c r="F53" s="11">
         <v>133798</v>
@@ -4091,7 +4048,7 @@
         <v>579</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>597</v>
+        <v>579</v>
       </c>
       <c r="F55" s="11">
         <v>7359</v>
@@ -4193,10 +4150,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D60" s="13" t="s">
+        <v>591</v>
+      </c>
+      <c r="E60" s="13" t="s">
         <v>590</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>705</v>
       </c>
       <c r="F60" s="11">
         <v>4307</v>
@@ -4298,10 +4255,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="F65" s="11">
         <v>12189</v>
@@ -4319,10 +4276,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>661</v>
+        <v>701</v>
       </c>
       <c r="F66" s="11">
         <v>171244</v>
@@ -4343,7 +4300,7 @@
         <v>579</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>644</v>
+        <v>618</v>
       </c>
       <c r="F67" s="11">
         <v>13454</v>
@@ -4361,10 +4318,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>689</v>
+        <v>702</v>
       </c>
       <c r="F68" s="11">
         <v>5520</v>
@@ -4448,7 +4405,7 @@
         <v>579</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>640</v>
+        <v>606</v>
       </c>
       <c r="F72" s="11">
         <v>7285</v>
@@ -4508,10 +4465,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>595</v>
+        <v>606</v>
       </c>
       <c r="F75" s="11">
         <v>32784</v>
@@ -4553,7 +4510,7 @@
         <v>579</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>595</v>
+        <v>680</v>
       </c>
       <c r="F77" s="11">
         <v>35892</v>
@@ -4574,7 +4531,7 @@
         <v>595</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>584</v>
+        <v>661</v>
       </c>
       <c r="F78" s="11">
         <v>17865</v>
@@ -4595,7 +4552,7 @@
         <v>579</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>644</v>
+        <v>588</v>
       </c>
       <c r="F79" s="11">
         <v>176376</v>
@@ -4616,7 +4573,7 @@
         <v>579</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>643</v>
+        <v>658</v>
       </c>
       <c r="F80" s="11">
         <v>6396</v>
@@ -4721,7 +4678,7 @@
         <v>596</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>586</v>
+        <v>703</v>
       </c>
       <c r="F85" s="11">
         <v>10216</v>
@@ -4739,10 +4696,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="F86" s="11">
         <v>25604</v>
@@ -4784,7 +4741,7 @@
         <v>597</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>681</v>
+        <v>686</v>
       </c>
       <c r="F88" s="11">
         <v>3114</v>
@@ -4847,7 +4804,7 @@
         <v>579</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>635</v>
+        <v>579</v>
       </c>
       <c r="F91" s="11">
         <v>10213</v>
@@ -4910,7 +4867,7 @@
         <v>598</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>613</v>
+        <v>658</v>
       </c>
       <c r="F94" s="11">
         <v>137452</v>
@@ -4931,7 +4888,7 @@
         <v>599</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>676</v>
+        <v>704</v>
       </c>
       <c r="F95" s="11">
         <v>65324</v>
@@ -4973,7 +4930,7 @@
         <v>579</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>700</v>
+        <v>623</v>
       </c>
       <c r="F97" s="11">
         <v>4472</v>
@@ -5036,7 +4993,7 @@
         <v>579</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>597</v>
+        <v>656</v>
       </c>
       <c r="F100" s="11">
         <v>209432</v>
@@ -5057,7 +5014,7 @@
         <v>579</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F101" s="11">
         <v>167408</v>
@@ -5141,7 +5098,7 @@
         <v>600</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>706</v>
+        <v>650</v>
       </c>
       <c r="F105" s="11">
         <v>133377</v>
@@ -5162,7 +5119,7 @@
         <v>579</v>
       </c>
       <c r="E106" s="13" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="F106" s="11">
         <v>18938</v>
@@ -5183,7 +5140,7 @@
         <v>601</v>
       </c>
       <c r="E107" s="13" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="F107" s="11">
         <v>110141</v>
@@ -5309,7 +5266,7 @@
         <v>602</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>671</v>
+        <v>596</v>
       </c>
       <c r="F113" s="11">
         <v>40017</v>
@@ -5351,7 +5308,7 @@
         <v>603</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="F115" s="11">
         <v>229059</v>
@@ -5411,10 +5368,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D118" s="13" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="E118" s="13" t="s">
-        <v>708</v>
+        <v>590</v>
       </c>
       <c r="F118" s="11">
         <v>5553</v>
@@ -5456,7 +5413,7 @@
         <v>604</v>
       </c>
       <c r="E120" s="13" t="s">
-        <v>703</v>
+        <v>629</v>
       </c>
       <c r="F120" s="11">
         <v>80193</v>
@@ -5624,7 +5581,7 @@
         <v>579</v>
       </c>
       <c r="E128" s="13" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="F128" s="11">
         <v>7566</v>
@@ -5645,7 +5602,7 @@
         <v>605</v>
       </c>
       <c r="E129" s="13" t="s">
-        <v>709</v>
+        <v>644</v>
       </c>
       <c r="F129" s="11">
         <v>62490</v>
@@ -5687,7 +5644,7 @@
         <v>579</v>
       </c>
       <c r="E131" s="13" t="s">
-        <v>710</v>
+        <v>676</v>
       </c>
       <c r="F131" s="11">
         <v>5625</v>
@@ -5705,10 +5662,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D132" s="13" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="E132" s="13" t="s">
-        <v>681</v>
+        <v>664</v>
       </c>
       <c r="F132" s="11">
         <v>65599</v>
@@ -5750,7 +5707,7 @@
         <v>579</v>
       </c>
       <c r="E134" s="13" t="s">
-        <v>666</v>
+        <v>706</v>
       </c>
       <c r="F134" s="11">
         <v>41492</v>
@@ -5771,7 +5728,7 @@
         <v>606</v>
       </c>
       <c r="E135" s="13" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="F135" s="11">
         <v>179317</v>
@@ -5792,7 +5749,7 @@
         <v>607</v>
       </c>
       <c r="E136" s="13" t="s">
-        <v>702</v>
+        <v>682</v>
       </c>
       <c r="F136" s="11">
         <v>50326</v>
@@ -5918,7 +5875,7 @@
         <v>608</v>
       </c>
       <c r="E142" s="13" t="s">
-        <v>643</v>
+        <v>680</v>
       </c>
       <c r="F142" s="11">
         <v>107523</v>
@@ -6020,10 +5977,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D147" s="13" t="s">
-        <v>609</v>
+        <v>590</v>
       </c>
       <c r="E147" s="13" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
       <c r="F147" s="11">
         <v>152935</v>
@@ -6044,7 +6001,7 @@
         <v>595</v>
       </c>
       <c r="E148" s="13" t="s">
-        <v>708</v>
+        <v>614</v>
       </c>
       <c r="F148" s="11">
         <v>171362</v>
@@ -6209,10 +6166,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D156" s="13" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E156" s="13" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="F156" s="11">
         <v>139021</v>
@@ -6251,10 +6208,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D158" s="13" t="s">
-        <v>585</v>
+        <v>610</v>
       </c>
       <c r="E158" s="13" t="s">
-        <v>710</v>
+        <v>686</v>
       </c>
       <c r="F158" s="11">
         <v>115844</v>
@@ -6293,10 +6250,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D160" s="13" t="s">
-        <v>611</v>
+        <v>584</v>
       </c>
       <c r="E160" s="13" t="s">
-        <v>591</v>
+        <v>692</v>
       </c>
       <c r="F160" s="11">
         <v>128766</v>
@@ -6377,10 +6334,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D164" s="13" t="s">
-        <v>612</v>
+        <v>585</v>
       </c>
       <c r="E164" s="13" t="s">
-        <v>611</v>
+        <v>697</v>
       </c>
       <c r="F164" s="11">
         <v>138053</v>
@@ -6482,10 +6439,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D169" s="13" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E169" s="13" t="s">
-        <v>712</v>
+        <v>641</v>
       </c>
       <c r="F169" s="11">
         <v>79604</v>
@@ -6566,10 +6523,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D173" s="13" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E173" s="13" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="F173" s="11">
         <v>136655</v>
@@ -6674,7 +6631,7 @@
         <v>579</v>
       </c>
       <c r="E178" s="13" t="s">
-        <v>666</v>
+        <v>579</v>
       </c>
       <c r="F178" s="11">
         <v>106558</v>
@@ -6713,10 +6670,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D180" s="13" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="E180" s="13" t="s">
-        <v>714</v>
+        <v>593</v>
       </c>
       <c r="F180" s="11">
         <v>79009</v>
@@ -6734,10 +6691,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D181" s="13" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="E181" s="13" t="s">
-        <v>613</v>
+        <v>658</v>
       </c>
       <c r="F181" s="11">
         <v>96377</v>
@@ -6755,10 +6712,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D182" s="13" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E182" s="13" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="F182" s="11">
         <v>168298</v>
@@ -6860,10 +6817,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D187" s="13" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E187" s="13" t="s">
-        <v>694</v>
+        <v>673</v>
       </c>
       <c r="F187" s="11">
         <v>171519</v>
@@ -6881,10 +6838,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D188" s="13" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E188" s="13" t="s">
-        <v>647</v>
+        <v>710</v>
       </c>
       <c r="F188" s="11">
         <v>108789</v>
@@ -6923,10 +6880,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D190" s="13" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="E190" s="13" t="s">
-        <v>661</v>
+        <v>617</v>
       </c>
       <c r="F190" s="11">
         <v>156305</v>
@@ -7070,10 +7027,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D197" s="13" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="E197" s="13" t="s">
-        <v>678</v>
+        <v>711</v>
       </c>
       <c r="F197" s="11">
         <v>102175</v>
@@ -7175,10 +7132,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D202" s="13" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E202" s="13" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="F202" s="11">
         <v>103900</v>
@@ -7367,7 +7324,7 @@
         <v>606</v>
       </c>
       <c r="E211" s="13" t="s">
-        <v>596</v>
+        <v>697</v>
       </c>
       <c r="F211" s="11">
         <v>149611</v>
@@ -7385,10 +7342,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D212" s="13" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E212" s="13" t="s">
-        <v>713</v>
+        <v>604</v>
       </c>
       <c r="F212" s="11">
         <v>180925</v>
@@ -7448,10 +7405,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D215" s="13" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E215" s="13" t="s">
-        <v>717</v>
+        <v>613</v>
       </c>
       <c r="F215" s="11">
         <v>90535</v>
@@ -7511,10 +7468,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D218" s="13" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="E218" s="13" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="F218" s="11">
         <v>768</v>
@@ -7574,10 +7531,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D221" s="13" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E221" s="13" t="s">
-        <v>697</v>
+        <v>613</v>
       </c>
       <c r="F221" s="11">
         <v>11003</v>
@@ -7679,10 +7636,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D226" s="13" t="s">
-        <v>591</v>
+        <v>622</v>
       </c>
       <c r="E226" s="13" t="s">
-        <v>614</v>
+        <v>688</v>
       </c>
       <c r="F226" s="11">
         <v>1033592</v>
@@ -7721,10 +7678,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D228" s="13" t="s">
-        <v>613</v>
+        <v>623</v>
       </c>
       <c r="E228" s="13" t="s">
-        <v>663</v>
+        <v>673</v>
       </c>
       <c r="F228" s="11">
         <v>79061</v>
@@ -7742,10 +7699,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D229" s="13" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="E229" s="13" t="s">
-        <v>628</v>
+        <v>605</v>
       </c>
       <c r="F229" s="11">
         <v>14053</v>
@@ -7784,10 +7741,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D231" s="13" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E231" s="13" t="s">
-        <v>719</v>
+        <v>666</v>
       </c>
       <c r="F231" s="11">
         <v>133038</v>
@@ -7826,10 +7783,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D233" s="13" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="E233" s="13" t="s">
-        <v>720</v>
+        <v>701</v>
       </c>
       <c r="F233" s="11">
         <v>24343</v>
@@ -7847,10 +7804,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D234" s="13" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E234" s="13" t="s">
-        <v>721</v>
+        <v>714</v>
       </c>
       <c r="F234" s="11">
         <v>21430</v>
@@ -7868,10 +7825,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D235" s="13" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E235" s="13" t="s">
-        <v>722</v>
+        <v>715</v>
       </c>
       <c r="F235" s="11">
         <v>9384</v>
@@ -7889,10 +7846,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D236" s="13" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E236" s="13" t="s">
-        <v>723</v>
+        <v>716</v>
       </c>
       <c r="F236" s="11">
         <v>841</v>
@@ -8015,10 +7972,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D242" s="13" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E242" s="13" t="s">
-        <v>619</v>
+        <v>717</v>
       </c>
       <c r="F242" s="11">
         <v>10354</v>
@@ -8078,10 +8035,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D245" s="13" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="E245" s="13" t="s">
-        <v>691</v>
+        <v>625</v>
       </c>
       <c r="F245" s="11">
         <v>88940</v>
@@ -8099,10 +8056,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D246" s="13" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E246" s="13" t="s">
-        <v>724</v>
+        <v>701</v>
       </c>
       <c r="F246" s="11">
         <v>48845</v>
@@ -8120,10 +8077,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D247" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E247" s="13" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="F247" s="11">
         <v>507632</v>
@@ -8144,7 +8101,7 @@
         <v>579</v>
       </c>
       <c r="E248" s="13" t="s">
-        <v>644</v>
+        <v>579</v>
       </c>
       <c r="F248" s="11">
         <v>8385</v>
@@ -8162,10 +8119,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D249" s="13" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="E249" s="13" t="s">
-        <v>726</v>
+        <v>647</v>
       </c>
       <c r="F249" s="11">
         <v>42934</v>
@@ -8183,10 +8140,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D250" s="13" t="s">
-        <v>635</v>
+        <v>579</v>
       </c>
       <c r="E250" s="13" t="s">
-        <v>637</v>
+        <v>614</v>
       </c>
       <c r="F250" s="11">
         <v>9092</v>
@@ -8225,10 +8182,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D252" s="13" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="E252" s="13" t="s">
-        <v>727</v>
+        <v>599</v>
       </c>
       <c r="F252" s="11">
         <v>169205</v>
@@ -8246,10 +8203,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D253" s="13" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="E253" s="13" t="s">
-        <v>728</v>
+        <v>627</v>
       </c>
       <c r="F253" s="11">
         <v>15572</v>
@@ -8288,10 +8245,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D255" s="13" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="E255" s="13" t="s">
-        <v>729</v>
+        <v>719</v>
       </c>
       <c r="F255" s="11">
         <v>30952</v>
@@ -8330,10 +8287,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D257" s="13" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="E257" s="13" t="s">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="F257" s="11">
         <v>33721</v>
@@ -8351,10 +8308,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D258" s="13" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="E258" s="13" t="s">
-        <v>642</v>
+        <v>721</v>
       </c>
       <c r="F258" s="11">
         <v>257354</v>
@@ -8393,10 +8350,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D260" s="13" t="s">
-        <v>640</v>
+        <v>581</v>
       </c>
       <c r="E260" s="13" t="s">
-        <v>727</v>
+        <v>688</v>
       </c>
       <c r="F260" s="11">
         <v>92238</v>
@@ -8456,10 +8413,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D263" s="13" t="s">
-        <v>641</v>
+        <v>580</v>
       </c>
       <c r="E263" s="13" t="s">
-        <v>600</v>
+        <v>678</v>
       </c>
       <c r="F263" s="11">
         <v>9851</v>
@@ -8477,10 +8434,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D264" s="13" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="E264" s="13" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
       <c r="F264" s="11">
         <v>18704</v>
@@ -8498,10 +8455,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D265" s="13" t="s">
-        <v>643</v>
+        <v>581</v>
       </c>
       <c r="E265" s="13" t="s">
-        <v>732</v>
+        <v>641</v>
       </c>
       <c r="F265" s="11">
         <v>372012</v>
@@ -8603,10 +8560,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D270" s="13" t="s">
-        <v>644</v>
+        <v>608</v>
       </c>
       <c r="E270" s="13" t="s">
-        <v>699</v>
+        <v>629</v>
       </c>
       <c r="F270" s="11">
         <v>47060</v>
@@ -8624,10 +8581,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D271" s="13" t="s">
-        <v>645</v>
+        <v>615</v>
       </c>
       <c r="E271" s="13" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
       <c r="F271" s="11">
         <v>8782</v>
@@ -8750,10 +8707,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D277" s="13" t="s">
-        <v>646</v>
+        <v>579</v>
       </c>
       <c r="E277" s="13" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="F277" s="11">
         <v>128912</v>
@@ -8792,10 +8749,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D279" s="13" t="s">
-        <v>647</v>
+        <v>614</v>
       </c>
       <c r="E279" s="13" t="s">
-        <v>734</v>
+        <v>701</v>
       </c>
       <c r="F279" s="11">
         <v>64482</v>
@@ -8813,10 +8770,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D280" s="13" t="s">
-        <v>648</v>
+        <v>637</v>
       </c>
       <c r="E280" s="13" t="s">
-        <v>735</v>
+        <v>724</v>
       </c>
       <c r="F280" s="11">
         <v>35027</v>
@@ -8834,10 +8791,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D281" s="13" t="s">
-        <v>649</v>
+        <v>630</v>
       </c>
       <c r="E281" s="13" t="s">
-        <v>642</v>
+        <v>725</v>
       </c>
       <c r="F281" s="11">
         <v>20963</v>
@@ -8855,10 +8812,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D282" s="13" t="s">
-        <v>650</v>
+        <v>614</v>
       </c>
       <c r="E282" s="13" t="s">
-        <v>736</v>
+        <v>679</v>
       </c>
       <c r="F282" s="11">
         <v>26417</v>
@@ -8876,10 +8833,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D283" s="13" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="E283" s="13" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="F283" s="11">
         <v>28960</v>
@@ -8897,10 +8854,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D284" s="13" t="s">
-        <v>651</v>
+        <v>638</v>
       </c>
       <c r="E284" s="13" t="s">
-        <v>691</v>
+        <v>673</v>
       </c>
       <c r="F284" s="11">
         <v>268741</v>
@@ -8918,10 +8875,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D285" s="13" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="E285" s="13" t="s">
-        <v>737</v>
+        <v>724</v>
       </c>
       <c r="F285" s="11">
         <v>20959</v>
@@ -8939,10 +8896,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D286" s="13" t="s">
-        <v>613</v>
+        <v>597</v>
       </c>
       <c r="E286" s="13" t="s">
-        <v>593</v>
+        <v>683</v>
       </c>
       <c r="F286" s="11">
         <v>134800</v>
@@ -9002,10 +8959,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D289" s="13" t="s">
-        <v>586</v>
+        <v>640</v>
       </c>
       <c r="E289" s="13" t="s">
-        <v>668</v>
+        <v>726</v>
       </c>
       <c r="F289" s="11">
         <v>156137</v>
@@ -9044,10 +9001,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D291" s="13" t="s">
-        <v>633</v>
+        <v>641</v>
       </c>
       <c r="E291" s="13" t="s">
-        <v>737</v>
+        <v>617</v>
       </c>
       <c r="F291" s="11">
         <v>26827</v>
@@ -9065,10 +9022,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D292" s="13" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="E292" s="13" t="s">
-        <v>738</v>
+        <v>727</v>
       </c>
       <c r="F292" s="11">
         <v>29012</v>
@@ -9149,10 +9106,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D296" s="13" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="E296" s="13" t="s">
-        <v>739</v>
+        <v>728</v>
       </c>
       <c r="F296" s="11">
         <v>1919</v>
@@ -9170,10 +9127,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D297" s="13" t="s">
-        <v>654</v>
+        <v>618</v>
       </c>
       <c r="E297" s="13" t="s">
-        <v>605</v>
+        <v>703</v>
       </c>
       <c r="F297" s="11">
         <v>24015</v>
@@ -9194,7 +9151,7 @@
         <v>579</v>
       </c>
       <c r="E298" s="13" t="s">
-        <v>621</v>
+        <v>579</v>
       </c>
       <c r="F298" s="11">
         <v>32450</v>
@@ -9212,10 +9169,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D299" s="13" t="s">
-        <v>655</v>
+        <v>644</v>
       </c>
       <c r="E299" s="13" t="s">
-        <v>740</v>
+        <v>729</v>
       </c>
       <c r="F299" s="11">
         <v>7450</v>
@@ -9233,10 +9190,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D300" s="13" t="s">
-        <v>582</v>
+        <v>596</v>
       </c>
       <c r="E300" s="13" t="s">
-        <v>593</v>
+        <v>688</v>
       </c>
       <c r="F300" s="11">
         <v>23281</v>
@@ -9275,10 +9232,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D302" s="13" t="s">
-        <v>598</v>
+        <v>579</v>
       </c>
       <c r="E302" s="13" t="s">
-        <v>741</v>
+        <v>654</v>
       </c>
       <c r="F302" s="11">
         <v>20392</v>
@@ -9296,10 +9253,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D303" s="13" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="E303" s="13" t="s">
-        <v>742</v>
+        <v>690</v>
       </c>
       <c r="F303" s="11">
         <v>2207</v>
@@ -9320,7 +9277,7 @@
         <v>579</v>
       </c>
       <c r="E304" s="13" t="s">
-        <v>743</v>
+        <v>629</v>
       </c>
       <c r="F304" s="11">
         <v>8879</v>
@@ -9362,7 +9319,7 @@
         <v>579</v>
       </c>
       <c r="E306" s="13" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="F306" s="11">
         <v>43509</v>
@@ -9401,10 +9358,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D308" s="13" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="E308" s="13" t="s">
-        <v>714</v>
+        <v>594</v>
       </c>
       <c r="F308" s="11">
         <v>100321</v>
@@ -9422,10 +9379,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D309" s="13" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="E309" s="13" t="s">
-        <v>744</v>
+        <v>586</v>
       </c>
       <c r="F309" s="11">
         <v>7775</v>
@@ -9485,10 +9442,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D312" s="13" t="s">
-        <v>644</v>
+        <v>581</v>
       </c>
       <c r="E312" s="13" t="s">
-        <v>690</v>
+        <v>730</v>
       </c>
       <c r="F312" s="11">
         <v>12687</v>
@@ -9527,10 +9484,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D314" s="13" t="s">
-        <v>656</v>
+        <v>584</v>
       </c>
       <c r="E314" s="13" t="s">
-        <v>719</v>
+        <v>726</v>
       </c>
       <c r="F314" s="11">
         <v>1418</v>
@@ -9572,7 +9529,7 @@
         <v>579</v>
       </c>
       <c r="E316" s="13" t="s">
-        <v>613</v>
+        <v>579</v>
       </c>
       <c r="F316" s="11">
         <v>19974</v>
@@ -9590,10 +9547,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D317" s="13" t="s">
-        <v>620</v>
+        <v>646</v>
       </c>
       <c r="E317" s="13" t="s">
-        <v>745</v>
+        <v>731</v>
       </c>
       <c r="F317" s="11">
         <v>3524</v>
@@ -9614,7 +9571,7 @@
         <v>579</v>
       </c>
       <c r="E318" s="13" t="s">
-        <v>580</v>
+        <v>606</v>
       </c>
       <c r="F318" s="11">
         <v>32295</v>
@@ -9653,10 +9610,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D320" s="13" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="E320" s="13" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="F320" s="11">
         <v>915</v>
@@ -9698,7 +9655,7 @@
         <v>579</v>
       </c>
       <c r="E322" s="13" t="s">
-        <v>617</v>
+        <v>708</v>
       </c>
       <c r="F322" s="11">
         <v>1982</v>
@@ -9716,10 +9673,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D323" s="13" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
       <c r="E323" s="13" t="s">
-        <v>746</v>
+        <v>733</v>
       </c>
       <c r="F323" s="11">
         <v>12222</v>
@@ -9758,10 +9715,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D325" s="13" t="s">
-        <v>659</v>
+        <v>624</v>
       </c>
       <c r="E325" s="13" t="s">
-        <v>614</v>
+        <v>631</v>
       </c>
       <c r="F325" s="11">
         <v>9682</v>
@@ -9800,10 +9757,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D327" s="13" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="E327" s="13" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
       <c r="F327" s="11">
         <v>77742</v>
@@ -9821,10 +9778,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D328" s="13" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
       <c r="E328" s="13" t="s">
-        <v>747</v>
+        <v>715</v>
       </c>
       <c r="F328" s="11">
         <v>7878</v>
@@ -9866,7 +9823,7 @@
         <v>579</v>
       </c>
       <c r="E330" s="13" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="F330" s="11">
         <v>29194</v>
@@ -9884,10 +9841,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D331" s="13" t="s">
-        <v>651</v>
+        <v>606</v>
       </c>
       <c r="E331" s="13" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F331" s="11">
         <v>28874</v>
@@ -9905,10 +9862,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D332" s="13" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="E332" s="13" t="s">
-        <v>748</v>
+        <v>613</v>
       </c>
       <c r="F332" s="11">
         <v>2491</v>
@@ -9926,10 +9883,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D333" s="13" t="s">
-        <v>661</v>
+        <v>646</v>
       </c>
       <c r="E333" s="13" t="s">
-        <v>749</v>
+        <v>734</v>
       </c>
       <c r="F333" s="11">
         <v>18602</v>
@@ -9950,7 +9907,7 @@
         <v>579</v>
       </c>
       <c r="E334" s="13" t="s">
-        <v>671</v>
+        <v>595</v>
       </c>
       <c r="F334" s="11">
         <v>6866</v>
@@ -9971,7 +9928,7 @@
         <v>579</v>
       </c>
       <c r="E335" s="13" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="F335" s="11">
         <v>3779</v>
@@ -9989,10 +9946,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D336" s="13" t="s">
-        <v>643</v>
+        <v>651</v>
       </c>
       <c r="E336" s="13" t="s">
-        <v>647</v>
+        <v>592</v>
       </c>
       <c r="F336" s="11">
         <v>31585</v>
@@ -10010,10 +9967,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D337" s="13" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
       <c r="E337" s="13" t="s">
-        <v>709</v>
+        <v>688</v>
       </c>
       <c r="F337" s="11">
         <v>140961</v>
@@ -10034,7 +9991,7 @@
         <v>579</v>
       </c>
       <c r="E338" s="13" t="s">
-        <v>594</v>
+        <v>618</v>
       </c>
       <c r="F338" s="11">
         <v>699</v>
@@ -10052,10 +10009,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D339" s="13" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="E339" s="13" t="s">
-        <v>717</v>
+        <v>736</v>
       </c>
       <c r="F339" s="11">
         <v>1470</v>
@@ -10073,10 +10030,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D340" s="13" t="s">
-        <v>664</v>
+        <v>639</v>
       </c>
       <c r="E340" s="13" t="s">
-        <v>750</v>
+        <v>650</v>
       </c>
       <c r="F340" s="11">
         <v>72425</v>
@@ -10094,10 +10051,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D341" s="13" t="s">
-        <v>590</v>
+        <v>611</v>
       </c>
       <c r="E341" s="13" t="s">
-        <v>614</v>
+        <v>631</v>
       </c>
       <c r="F341" s="11">
         <v>105880</v>
@@ -10115,10 +10072,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D342" s="13" t="s">
-        <v>665</v>
+        <v>654</v>
       </c>
       <c r="E342" s="13" t="s">
-        <v>629</v>
+        <v>724</v>
       </c>
       <c r="F342" s="11">
         <v>11206</v>
@@ -10157,10 +10114,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D344" s="13" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E344" s="13" t="s">
-        <v>661</v>
+        <v>612</v>
       </c>
       <c r="F344" s="11">
         <v>14441</v>
@@ -10178,10 +10135,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D345" s="13" t="s">
-        <v>666</v>
+        <v>579</v>
       </c>
       <c r="E345" s="13" t="s">
-        <v>674</v>
+        <v>584</v>
       </c>
       <c r="F345" s="11">
         <v>17667</v>
@@ -10202,7 +10159,7 @@
         <v>579</v>
       </c>
       <c r="E346" s="13" t="s">
-        <v>699</v>
+        <v>737</v>
       </c>
       <c r="F346" s="11">
         <v>8204</v>
@@ -10223,7 +10180,7 @@
         <v>579</v>
       </c>
       <c r="E347" s="13" t="s">
-        <v>681</v>
+        <v>606</v>
       </c>
       <c r="F347" s="11">
         <v>1263</v>
@@ -10262,10 +10219,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D349" s="13" t="s">
-        <v>641</v>
+        <v>590</v>
       </c>
       <c r="E349" s="13" t="s">
-        <v>751</v>
+        <v>726</v>
       </c>
       <c r="F349" s="11">
         <v>114763</v>
@@ -10325,10 +10282,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D352" s="13" t="s">
-        <v>626</v>
+        <v>654</v>
       </c>
       <c r="E352" s="13" t="s">
-        <v>614</v>
+        <v>678</v>
       </c>
       <c r="F352" s="11">
         <v>5557</v>
@@ -10346,10 +10303,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D353" s="13" t="s">
-        <v>612</v>
+        <v>656</v>
       </c>
       <c r="E353" s="13" t="s">
-        <v>649</v>
+        <v>682</v>
       </c>
       <c r="F353" s="11">
         <v>82506</v>
@@ -10367,10 +10324,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D354" s="13" t="s">
-        <v>631</v>
+        <v>657</v>
       </c>
       <c r="E354" s="13" t="s">
-        <v>628</v>
+        <v>617</v>
       </c>
       <c r="F354" s="11">
         <v>4457</v>
@@ -10409,10 +10366,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D356" s="13" t="s">
-        <v>602</v>
+        <v>658</v>
       </c>
       <c r="E356" s="13" t="s">
-        <v>674</v>
+        <v>622</v>
       </c>
       <c r="F356" s="11">
         <v>32926</v>
@@ -10433,7 +10390,7 @@
         <v>579</v>
       </c>
       <c r="E357" s="13" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="F357" s="11">
         <v>13395</v>
@@ -10451,10 +10408,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D358" s="13" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="E358" s="13" t="s">
-        <v>668</v>
+        <v>738</v>
       </c>
       <c r="F358" s="11">
         <v>5537</v>
@@ -10472,10 +10429,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D359" s="13" t="s">
-        <v>635</v>
+        <v>579</v>
       </c>
       <c r="E359" s="13" t="s">
-        <v>596</v>
+        <v>686</v>
       </c>
       <c r="F359" s="11">
         <v>6778</v>
@@ -10493,10 +10450,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D360" s="13" t="s">
-        <v>615</v>
+        <v>660</v>
       </c>
       <c r="E360" s="13" t="s">
-        <v>647</v>
+        <v>691</v>
       </c>
       <c r="F360" s="11">
         <v>9916</v>
@@ -10514,10 +10471,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D361" s="13" t="s">
-        <v>609</v>
+        <v>661</v>
       </c>
       <c r="E361" s="13" t="s">
-        <v>655</v>
+        <v>678</v>
       </c>
       <c r="F361" s="11">
         <v>51839</v>
@@ -10535,10 +10492,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D362" s="13" t="s">
-        <v>605</v>
+        <v>662</v>
       </c>
       <c r="E362" s="13" t="s">
-        <v>752</v>
+        <v>647</v>
       </c>
       <c r="F362" s="11">
         <v>17494</v>
@@ -10577,10 +10534,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D364" s="13" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="E364" s="13" t="s">
-        <v>732</v>
+        <v>659</v>
       </c>
       <c r="F364" s="11">
         <v>4774</v>
@@ -10598,10 +10555,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D365" s="13" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="E365" s="13" t="s">
-        <v>634</v>
+        <v>586</v>
       </c>
       <c r="F365" s="11">
         <v>9738</v>
@@ -10640,10 +10597,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D367" s="13" t="s">
-        <v>625</v>
+        <v>588</v>
       </c>
       <c r="E367" s="13" t="s">
-        <v>620</v>
+        <v>739</v>
       </c>
       <c r="F367" s="11">
         <v>31107</v>
@@ -10661,10 +10618,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D368" s="13" t="s">
-        <v>641</v>
+        <v>664</v>
       </c>
       <c r="E368" s="13" t="s">
-        <v>657</v>
+        <v>724</v>
       </c>
       <c r="F368" s="11">
         <v>69570</v>
@@ -10703,10 +10660,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D370" s="13" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="E370" s="13" t="s">
-        <v>673</v>
+        <v>594</v>
       </c>
       <c r="F370" s="11">
         <v>12635</v>
@@ -10724,10 +10681,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D371" s="13" t="s">
-        <v>641</v>
+        <v>596</v>
       </c>
       <c r="E371" s="13" t="s">
-        <v>719</v>
+        <v>740</v>
       </c>
       <c r="F371" s="11">
         <v>12975</v>
@@ -10745,10 +10702,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D372" s="13" t="s">
-        <v>627</v>
+        <v>641</v>
       </c>
       <c r="E372" s="13" t="s">
-        <v>753</v>
+        <v>724</v>
       </c>
       <c r="F372" s="11">
         <v>57472</v>
@@ -10766,10 +10723,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D373" s="13" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="E373" s="13" t="s">
-        <v>754</v>
+        <v>736</v>
       </c>
       <c r="F373" s="11">
         <v>35165</v>
@@ -10787,10 +10744,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D374" s="13" t="s">
-        <v>599</v>
+        <v>666</v>
       </c>
       <c r="E374" s="13" t="s">
-        <v>755</v>
+        <v>685</v>
       </c>
       <c r="F374" s="11">
         <v>1498</v>
@@ -10808,10 +10765,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D375" s="13" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E375" s="13" t="s">
-        <v>756</v>
+        <v>741</v>
       </c>
       <c r="F375" s="11">
         <v>1453</v>
@@ -10829,10 +10786,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D376" s="13" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E376" s="13" t="s">
-        <v>757</v>
+        <v>742</v>
       </c>
       <c r="F376" s="11">
         <v>1420</v>
@@ -10853,7 +10810,7 @@
         <v>579</v>
       </c>
       <c r="E377" s="13" t="s">
-        <v>696</v>
+        <v>673</v>
       </c>
       <c r="F377" s="11">
         <v>3882</v>
@@ -10871,10 +10828,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D378" s="13" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="E378" s="13" t="s">
-        <v>669</v>
+        <v>633</v>
       </c>
       <c r="F378" s="11">
         <v>759</v>
@@ -10913,10 +10870,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D380" s="13" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E380" s="13" t="s">
-        <v>758</v>
+        <v>743</v>
       </c>
       <c r="F380" s="11">
         <v>827</v>
@@ -10958,7 +10915,7 @@
         <v>579</v>
       </c>
       <c r="E382" s="13" t="s">
-        <v>691</v>
+        <v>744</v>
       </c>
       <c r="F382" s="11">
         <v>25968</v>
@@ -10976,10 +10933,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D383" s="13" t="s">
-        <v>621</v>
+        <v>579</v>
       </c>
       <c r="E383" s="13" t="s">
-        <v>759</v>
+        <v>688</v>
       </c>
       <c r="F383" s="11">
         <v>31743</v>
@@ -11000,7 +10957,7 @@
         <v>579</v>
       </c>
       <c r="E384" s="13" t="s">
-        <v>635</v>
+        <v>579</v>
       </c>
       <c r="F384" s="11">
         <v>22905</v>
@@ -11021,7 +10978,7 @@
         <v>579</v>
       </c>
       <c r="E385" s="13" t="s">
-        <v>591</v>
+        <v>697</v>
       </c>
       <c r="F385" s="11">
         <v>76082</v>
@@ -11039,10 +10996,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D386" s="13" t="s">
-        <v>671</v>
+        <v>606</v>
       </c>
       <c r="E386" s="13" t="s">
-        <v>716</v>
+        <v>745</v>
       </c>
       <c r="F386" s="11">
         <v>14004</v>
@@ -11102,10 +11059,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D389" s="13" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E389" s="13" t="s">
-        <v>760</v>
+        <v>746</v>
       </c>
       <c r="F389" s="11">
         <v>1179</v>
@@ -11123,10 +11080,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D390" s="13" t="s">
-        <v>673</v>
+        <v>615</v>
       </c>
       <c r="E390" s="13" t="s">
-        <v>761</v>
+        <v>747</v>
       </c>
       <c r="F390" s="11">
         <v>4799</v>
@@ -11147,7 +11104,7 @@
         <v>579</v>
       </c>
       <c r="E391" s="13" t="s">
-        <v>615</v>
+        <v>579</v>
       </c>
       <c r="F391" s="11">
         <v>9016</v>
@@ -11165,10 +11122,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D392" s="13" t="s">
-        <v>674</v>
+        <v>590</v>
       </c>
       <c r="E392" s="13" t="s">
-        <v>725</v>
+        <v>609</v>
       </c>
       <c r="F392" s="11">
         <v>91462</v>
@@ -11186,10 +11143,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D393" s="13" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E393" s="13" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="F393" s="11">
         <v>6971</v>
@@ -11207,10 +11164,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D394" s="13" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="E394" s="13" t="s">
-        <v>762</v>
+        <v>748</v>
       </c>
       <c r="F394" s="11">
         <v>2660</v>
@@ -11228,10 +11185,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D395" s="13" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="E395" s="13" t="s">
-        <v>754</v>
+        <v>723</v>
       </c>
       <c r="F395" s="11">
         <v>836</v>
@@ -11291,10 +11248,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D398" s="13" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="E398" s="13" t="s">
-        <v>616</v>
+        <v>749</v>
       </c>
       <c r="F398" s="11">
         <v>846</v>
@@ -11312,10 +11269,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D399" s="13" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="E399" s="13" t="s">
-        <v>763</v>
+        <v>733</v>
       </c>
       <c r="F399" s="11">
         <v>707</v>
@@ -11354,10 +11311,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D401" s="13" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="E401" s="13" t="s">
-        <v>764</v>
+        <v>750</v>
       </c>
       <c r="F401" s="11">
         <v>1138</v>
@@ -11396,10 +11353,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D403" s="13" t="s">
-        <v>621</v>
+        <v>579</v>
       </c>
       <c r="E403" s="13" t="s">
-        <v>696</v>
+        <v>642</v>
       </c>
       <c r="F403" s="11">
         <v>2759</v>
@@ -11417,10 +11374,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D404" s="13" t="s">
-        <v>607</v>
+        <v>580</v>
       </c>
       <c r="E404" s="13" t="s">
-        <v>753</v>
+        <v>725</v>
       </c>
       <c r="F404" s="11">
         <v>11258</v>
@@ -11438,10 +11395,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D405" s="13" t="s">
-        <v>599</v>
+        <v>631</v>
       </c>
       <c r="E405" s="13" t="s">
-        <v>749</v>
+        <v>731</v>
       </c>
       <c r="F405" s="11">
         <v>5119</v>
@@ -11480,10 +11437,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D407" s="13" t="s">
-        <v>680</v>
+        <v>624</v>
       </c>
       <c r="E407" s="13" t="s">
-        <v>765</v>
+        <v>621</v>
       </c>
       <c r="F407" s="11">
         <v>4989</v>
@@ -11504,7 +11461,7 @@
         <v>579</v>
       </c>
       <c r="E408" s="13" t="s">
-        <v>766</v>
+        <v>691</v>
       </c>
       <c r="F408" s="11">
         <v>508</v>
@@ -11564,10 +11521,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D411" s="13" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="E411" s="13" t="s">
-        <v>699</v>
+        <v>751</v>
       </c>
       <c r="F411" s="11">
         <v>6394</v>
@@ -11651,7 +11608,7 @@
         <v>579</v>
       </c>
       <c r="E415" s="13" t="s">
-        <v>631</v>
+        <v>592</v>
       </c>
       <c r="F415" s="11">
         <v>26450</v>
@@ -11669,10 +11626,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D416" s="13" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="E416" s="13" t="s">
-        <v>727</v>
+        <v>690</v>
       </c>
       <c r="F416" s="11">
         <v>4484</v>
@@ -11711,10 +11668,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D418" s="13" t="s">
-        <v>683</v>
+        <v>603</v>
       </c>
       <c r="E418" s="13" t="s">
-        <v>767</v>
+        <v>752</v>
       </c>
       <c r="F418" s="11">
         <v>801</v>
@@ -11732,10 +11689,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D419" s="13" t="s">
-        <v>684</v>
+        <v>584</v>
       </c>
       <c r="E419" s="13" t="s">
-        <v>657</v>
+        <v>738</v>
       </c>
       <c r="F419" s="11">
         <v>97821</v>
@@ -11756,7 +11713,7 @@
         <v>579</v>
       </c>
       <c r="E420" s="13" t="s">
-        <v>610</v>
+        <v>599</v>
       </c>
       <c r="F420" s="11">
         <v>30224</v>
@@ -11795,10 +11752,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D422" s="13" t="s">
-        <v>685</v>
+        <v>579</v>
       </c>
       <c r="E422" s="13" t="s">
-        <v>768</v>
+        <v>599</v>
       </c>
       <c r="F422" s="11">
         <v>21919</v>
@@ -11819,7 +11776,7 @@
         <v>579</v>
       </c>
       <c r="E423" s="13" t="s">
-        <v>694</v>
+        <v>590</v>
       </c>
       <c r="F423" s="11">
         <v>2968</v>
@@ -11861,7 +11818,7 @@
         <v>579</v>
       </c>
       <c r="E425" s="13" t="s">
-        <v>741</v>
+        <v>614</v>
       </c>
       <c r="F425" s="11">
         <v>128904</v>
@@ -11879,10 +11836,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D426" s="13" t="s">
-        <v>681</v>
+        <v>601</v>
       </c>
       <c r="E426" s="13" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="F426" s="11">
         <v>47402</v>
@@ -11900,10 +11857,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D427" s="13" t="s">
-        <v>686</v>
+        <v>614</v>
       </c>
       <c r="E427" s="13" t="s">
-        <v>769</v>
+        <v>753</v>
       </c>
       <c r="F427" s="11">
         <v>22664</v>
@@ -11942,10 +11899,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D429" s="13" t="s">
-        <v>621</v>
+        <v>660</v>
       </c>
       <c r="E429" s="13" t="s">
-        <v>753</v>
+        <v>593</v>
       </c>
       <c r="F429" s="11">
         <v>3176</v>
@@ -11963,10 +11920,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D430" s="13" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="E430" s="13" t="s">
-        <v>770</v>
+        <v>720</v>
       </c>
       <c r="F430" s="11">
         <v>979</v>
@@ -12089,10 +12046,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D436" s="13" t="s">
-        <v>648</v>
+        <v>633</v>
       </c>
       <c r="E436" s="13" t="s">
-        <v>745</v>
+        <v>754</v>
       </c>
       <c r="F436" s="11">
         <v>34833</v>
@@ -12176,7 +12133,7 @@
         <v>579</v>
       </c>
       <c r="E440" s="13" t="s">
-        <v>759</v>
+        <v>662</v>
       </c>
       <c r="F440" s="11">
         <v>70627</v>
@@ -12197,7 +12154,7 @@
         <v>579</v>
       </c>
       <c r="E441" s="13" t="s">
-        <v>771</v>
+        <v>587</v>
       </c>
       <c r="F441" s="11">
         <v>7424</v>
@@ -12239,7 +12196,7 @@
         <v>579</v>
       </c>
       <c r="E443" s="13" t="s">
-        <v>641</v>
+        <v>596</v>
       </c>
       <c r="F443" s="11">
         <v>84438</v>
@@ -12278,10 +12235,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D445" s="13" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="E445" s="13" t="s">
-        <v>772</v>
+        <v>755</v>
       </c>
       <c r="F445" s="11">
         <v>2715</v>
@@ -12323,7 +12280,7 @@
         <v>579</v>
       </c>
       <c r="E447" s="13" t="s">
-        <v>703</v>
+        <v>604</v>
       </c>
       <c r="F447" s="11">
         <v>1842</v>
@@ -12362,10 +12319,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D449" s="13" t="s">
-        <v>651</v>
+        <v>680</v>
       </c>
       <c r="E449" s="13" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
       <c r="F449" s="11">
         <v>7601</v>
@@ -12446,10 +12403,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D453" s="13" t="s">
-        <v>641</v>
+        <v>681</v>
       </c>
       <c r="E453" s="13" t="s">
-        <v>725</v>
+        <v>756</v>
       </c>
       <c r="F453" s="11">
         <v>32172</v>
@@ -12488,10 +12445,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D455" s="13" t="s">
-        <v>647</v>
+        <v>682</v>
       </c>
       <c r="E455" s="13" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="F455" s="11">
         <v>14573</v>
@@ -12509,10 +12466,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D456" s="13" t="s">
-        <v>625</v>
+        <v>588</v>
       </c>
       <c r="E456" s="13" t="s">
-        <v>618</v>
+        <v>666</v>
       </c>
       <c r="F456" s="11">
         <v>1149</v>
@@ -12551,10 +12508,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D458" s="13" t="s">
-        <v>664</v>
+        <v>683</v>
       </c>
       <c r="E458" s="13" t="s">
-        <v>773</v>
+        <v>738</v>
       </c>
       <c r="F458" s="11">
         <v>4023</v>
@@ -12614,10 +12571,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D461" s="13" t="s">
-        <v>618</v>
+        <v>684</v>
       </c>
       <c r="E461" s="13" t="s">
-        <v>707</v>
+        <v>758</v>
       </c>
       <c r="F461" s="11">
         <v>9004</v>
@@ -12677,10 +12634,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D464" s="13" t="s">
-        <v>657</v>
+        <v>685</v>
       </c>
       <c r="E464" s="13" t="s">
-        <v>670</v>
+        <v>759</v>
       </c>
       <c r="F464" s="11">
         <v>1470</v>
@@ -12719,10 +12676,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D466" s="13" t="s">
-        <v>640</v>
+        <v>651</v>
       </c>
       <c r="E466" s="13" t="s">
-        <v>774</v>
+        <v>684</v>
       </c>
       <c r="F466" s="11">
         <v>26749</v>
@@ -12740,10 +12697,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D467" s="13" t="s">
-        <v>688</v>
+        <v>579</v>
       </c>
       <c r="E467" s="13" t="s">
-        <v>744</v>
+        <v>630</v>
       </c>
       <c r="F467" s="11">
         <v>919</v>
@@ -12761,10 +12718,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D468" s="13" t="s">
-        <v>656</v>
+        <v>686</v>
       </c>
       <c r="E468" s="13" t="s">
-        <v>629</v>
+        <v>617</v>
       </c>
       <c r="F468" s="11">
         <v>4330</v>
@@ -12803,10 +12760,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D470" s="13" t="s">
-        <v>621</v>
+        <v>598</v>
       </c>
       <c r="E470" s="13" t="s">
-        <v>619</v>
+        <v>760</v>
       </c>
       <c r="F470" s="11">
         <v>808</v>
@@ -12845,10 +12802,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D472" s="13" t="s">
-        <v>664</v>
+        <v>640</v>
       </c>
       <c r="E472" s="13" t="s">
-        <v>720</v>
+        <v>761</v>
       </c>
       <c r="F472" s="11">
         <v>105754</v>
@@ -12887,10 +12844,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D474" s="13" t="s">
-        <v>689</v>
+        <v>672</v>
       </c>
       <c r="E474" s="13" t="s">
-        <v>775</v>
+        <v>762</v>
       </c>
       <c r="F474" s="11">
         <v>24591</v>
@@ -12929,10 +12886,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D476" s="13" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="E476" s="13" t="s">
-        <v>711</v>
+        <v>600</v>
       </c>
       <c r="F476" s="11">
         <v>37440</v>
@@ -12950,10 +12907,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D477" s="13" t="s">
-        <v>686</v>
+        <v>614</v>
       </c>
       <c r="E477" s="13" t="s">
-        <v>624</v>
+        <v>740</v>
       </c>
       <c r="F477" s="11">
         <v>183276</v>
@@ -12971,10 +12928,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D478" s="13" t="s">
-        <v>598</v>
+        <v>660</v>
       </c>
       <c r="E478" s="13" t="s">
-        <v>617</v>
+        <v>582</v>
       </c>
       <c r="F478" s="11">
         <v>14512</v>
@@ -12992,10 +12949,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D479" s="13" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
       <c r="E479" s="13" t="s">
-        <v>706</v>
+        <v>756</v>
       </c>
       <c r="F479" s="11">
         <v>114972</v>
@@ -13016,7 +12973,7 @@
         <v>579</v>
       </c>
       <c r="E480" s="13" t="s">
-        <v>680</v>
+        <v>696</v>
       </c>
       <c r="F480" s="11">
         <v>303</v>
@@ -13055,10 +13012,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D482" s="13" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="E482" s="13" t="s">
-        <v>683</v>
+        <v>731</v>
       </c>
       <c r="F482" s="11">
         <v>3851</v>
@@ -13118,10 +13075,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D485" s="13" t="s">
-        <v>669</v>
+        <v>689</v>
       </c>
       <c r="E485" s="13" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F485" s="11">
         <v>31968</v>
@@ -13139,10 +13096,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D486" s="13" t="s">
-        <v>692</v>
+        <v>662</v>
       </c>
       <c r="E486" s="13" t="s">
-        <v>754</v>
+        <v>763</v>
       </c>
       <c r="F486" s="11">
         <v>750</v>
@@ -13160,10 +13117,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D487" s="13" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="E487" s="13" t="s">
-        <v>737</v>
+        <v>764</v>
       </c>
       <c r="F487" s="11">
         <v>31265</v>
@@ -13181,10 +13138,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D488" s="13" t="s">
-        <v>584</v>
+        <v>655</v>
       </c>
       <c r="E488" s="13" t="s">
-        <v>768</v>
+        <v>684</v>
       </c>
       <c r="F488" s="11">
         <v>1482</v>
@@ -13202,10 +13159,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D489" s="13" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E489" s="13" t="s">
-        <v>776</v>
+        <v>704</v>
       </c>
       <c r="F489" s="11">
         <v>348</v>
@@ -13223,10 +13180,10 @@
         <v>Major Cities of Australia</v>
       </c>
       <c r="D490" s="13" t="s">
-        <v>695</v>
+        <v>673</v>
       </c>
       <c r="E490" s="13" t="s">
-        <v>622</v>
+        <v>720</v>
       </c>
       <c r="F490" s="11">
         <v>161346</v>
@@ -13244,10 +13201,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D491" s="13" t="s">
-        <v>627</v>
+        <v>692</v>
       </c>
       <c r="E491" s="13" t="s">
-        <v>670</v>
+        <v>648</v>
       </c>
       <c r="F491" s="11">
         <v>3452</v>
@@ -13265,10 +13222,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D492" s="13" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E492" s="13" t="s">
-        <v>734</v>
+        <v>749</v>
       </c>
       <c r="F492" s="11">
         <v>624</v>
@@ -13310,7 +13267,7 @@
         <v>579</v>
       </c>
       <c r="E494" s="13" t="s">
-        <v>705</v>
+        <v>664</v>
       </c>
       <c r="F494" s="11">
         <v>556</v>
@@ -13328,10 +13285,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D495" s="13" t="s">
-        <v>588</v>
+        <v>656</v>
       </c>
       <c r="E495" s="13" t="s">
-        <v>599</v>
+        <v>765</v>
       </c>
       <c r="F495" s="11">
         <v>784</v>
@@ -13373,7 +13330,7 @@
         <v>579</v>
       </c>
       <c r="E497" s="13" t="s">
-        <v>777</v>
+        <v>601</v>
       </c>
       <c r="F497" s="11">
         <v>1002</v>
@@ -13391,10 +13348,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D498" s="13" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="E498" s="13" t="s">
-        <v>778</v>
+        <v>766</v>
       </c>
       <c r="F498" s="11">
         <v>335</v>
@@ -13412,10 +13369,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D499" s="13" t="s">
-        <v>698</v>
+        <v>614</v>
       </c>
       <c r="E499" s="13" t="s">
-        <v>779</v>
+        <v>727</v>
       </c>
       <c r="F499" s="11">
         <v>422</v>
@@ -13496,10 +13453,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D503" s="13" t="s">
-        <v>647</v>
+        <v>629</v>
       </c>
       <c r="E503" s="13" t="s">
-        <v>658</v>
+        <v>707</v>
       </c>
       <c r="F503" s="11">
         <v>2974</v>
@@ -13520,7 +13477,7 @@
         <v>579</v>
       </c>
       <c r="E504" s="13" t="s">
-        <v>647</v>
+        <v>692</v>
       </c>
       <c r="F504" s="11">
         <v>5386</v>
@@ -13541,7 +13498,7 @@
         <v>579</v>
       </c>
       <c r="E505" s="13" t="s">
-        <v>680</v>
+        <v>663</v>
       </c>
       <c r="F505" s="11">
         <v>13587</v>
@@ -13559,10 +13516,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D506" s="13" t="s">
-        <v>643</v>
+        <v>656</v>
       </c>
       <c r="E506" s="13" t="s">
-        <v>780</v>
+        <v>665</v>
       </c>
       <c r="F506" s="11">
         <v>15920</v>
@@ -13583,7 +13540,7 @@
         <v>579</v>
       </c>
       <c r="E507" s="13" t="s">
-        <v>712</v>
+        <v>590</v>
       </c>
       <c r="F507" s="11">
         <v>18315</v>
@@ -13601,10 +13558,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D508" s="13" t="s">
-        <v>643</v>
+        <v>581</v>
       </c>
       <c r="E508" s="13" t="s">
-        <v>732</v>
+        <v>633</v>
       </c>
       <c r="F508" s="11">
         <v>1767</v>
@@ -13622,10 +13579,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D509" s="13" t="s">
-        <v>587</v>
+        <v>673</v>
       </c>
       <c r="E509" s="13" t="s">
-        <v>753</v>
+        <v>767</v>
       </c>
       <c r="F509" s="11">
         <v>6433</v>
@@ -13667,7 +13624,7 @@
         <v>579</v>
       </c>
       <c r="E511" s="13" t="s">
-        <v>664</v>
+        <v>691</v>
       </c>
       <c r="F511" s="11">
         <v>8478</v>
@@ -13688,7 +13645,7 @@
         <v>579</v>
       </c>
       <c r="E512" s="13" t="s">
-        <v>587</v>
+        <v>737</v>
       </c>
       <c r="F512" s="11">
         <v>20988</v>
@@ -13706,10 +13663,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D513" s="13" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E513" s="13" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="F513" s="11">
         <v>5525</v>
@@ -13748,10 +13705,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D515" s="13" t="s">
-        <v>650</v>
+        <v>695</v>
       </c>
       <c r="E515" s="13" t="s">
-        <v>742</v>
+        <v>615</v>
       </c>
       <c r="F515" s="11">
         <v>5764</v>
@@ -13832,10 +13789,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D519" s="13" t="s">
-        <v>595</v>
+        <v>696</v>
       </c>
       <c r="E519" s="13" t="s">
-        <v>605</v>
+        <v>645</v>
       </c>
       <c r="F519" s="11">
         <v>14405</v>
@@ -13853,10 +13810,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D520" s="13" t="s">
-        <v>699</v>
+        <v>657</v>
       </c>
       <c r="E520" s="13" t="s">
-        <v>781</v>
+        <v>701</v>
       </c>
       <c r="F520" s="11">
         <v>5322</v>
@@ -13916,10 +13873,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D523" s="13" t="s">
-        <v>700</v>
+        <v>579</v>
       </c>
       <c r="E523" s="13" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="F523" s="11">
         <v>9713</v>
@@ -13940,7 +13897,7 @@
         <v>579</v>
       </c>
       <c r="E524" s="13" t="s">
-        <v>665</v>
+        <v>596</v>
       </c>
       <c r="F524" s="11">
         <v>55869</v>
@@ -13958,10 +13915,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D525" s="13" t="s">
-        <v>580</v>
+        <v>606</v>
       </c>
       <c r="E525" s="13" t="s">
-        <v>732</v>
+        <v>633</v>
       </c>
       <c r="F525" s="11">
         <v>16467</v>
@@ -13979,10 +13936,10 @@
         <v>Inner Regional Australia</v>
       </c>
       <c r="D526" s="13" t="s">
-        <v>700</v>
+        <v>579</v>
       </c>
       <c r="E526" s="13" t="s">
-        <v>647</v>
+        <v>614</v>
       </c>
       <c r="F526" s="11">
         <v>11170</v>
@@ -14003,7 +13960,7 @@
         <v>579</v>
       </c>
       <c r="E527" s="13" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
       <c r="F527" s="11">
         <v>12763</v>
@@ -14021,10 +13978,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D528" s="13" t="s">
-        <v>656</v>
+        <v>697</v>
       </c>
       <c r="E528" s="13" t="s">
-        <v>655</v>
+        <v>684</v>
       </c>
       <c r="F528" s="11">
         <v>5144</v>
@@ -14045,7 +14002,7 @@
         <v>579</v>
       </c>
       <c r="E529" s="13" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="F529" s="11">
         <v>2135</v>
@@ -14063,10 +14020,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D530" s="13" t="s">
-        <v>606</v>
+        <v>585</v>
       </c>
       <c r="E530" s="13" t="s">
-        <v>599</v>
+        <v>662</v>
       </c>
       <c r="F530" s="11">
         <v>11370</v>
@@ -14108,7 +14065,7 @@
         <v>579</v>
       </c>
       <c r="E532" s="13" t="s">
-        <v>671</v>
+        <v>606</v>
       </c>
       <c r="F532" s="11">
         <v>19931</v>
@@ -14294,10 +14251,10 @@
         <v>Outer Regional Australia</v>
       </c>
       <c r="D541" s="13" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="E541" s="13" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="F541" s="11">
         <v>21345</v>
@@ -14339,7 +14296,7 @@
         <v>579</v>
       </c>
       <c r="E543" s="13" t="s">
-        <v>662</v>
+        <v>680</v>
       </c>
       <c r="F543" s="11">
         <v>28583</v>
@@ -16185,24 +16142,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB2B734-64E5-46B2-992B-E3CED3E06B45}">
-  <dimension ref="A1:I546"/>
+  <dimension ref="A1:B546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A443" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B546" sqref="A1:B546"/>
-    </sheetView>
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" hidden="1"/>
-    <col min="4" max="4" width="33" hidden="1"/>
-    <col min="5" max="5" width="20" hidden="1"/>
-    <col min="6" max="6" width="14.28515625" hidden="1"/>
-    <col min="7" max="7" width="19.85546875" hidden="1"/>
-    <col min="8" max="8" width="20.42578125" hidden="1"/>
-    <col min="9" max="9" width="16" hidden="1"/>
-    <col min="10" max="16384" width="9.140625" hidden="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -20565,7 +20518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="546" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A546" s="8" t="s">
         <v>563</v>
       </c>

</xml_diff>